<commit_message>
update view and action in wire frame
</commit_message>
<xml_diff>
--- a/shipping-cost.xlsx
+++ b/shipping-cost.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Fedex</t>
   </si>
@@ -91,12 +91,17 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Disclaimers:
+·       Customs duties, taxes, service charges and clearance related charges and any other fees (where applicable) are not included in the tariffs.
+·       Freight rates effective for the current calendar year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,12 +147,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +168,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -205,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +725,21 @@
         <v>1009</v>
       </c>
     </row>
+    <row r="13" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B13:H13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>